<commit_message>
SRG prep, new computer
I did some initial (probably trash) analyses prior to the 2024 PSRG meeting. This is also the first commit from my new computer, which requires an update to all repos.
</commit_message>
<xml_diff>
--- a/results-raw/sample.performance.across.all.runs.xlsx
+++ b/results-raw/sample.performance.across.all.runs.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,20 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/KKMDocuments/Documents/Github.Repos/Mnov/Mnov.gtseq.analysis/results-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{33AC7C9C-B259-5D4E-A419-A81424ABAA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF767FB-BBA3-744D-ABC0-1E866D7DA231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16660" yWindow="500" windowWidth="26840" windowHeight="15940"/>
+    <workbookView xWindow="37480" yWindow="4860" windowWidth="26840" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample.performance.across.all.r" sheetId="1" r:id="rId1"/>
     <sheet name="cannot compare" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5187" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5201" uniqueCount="796">
   <si>
     <t>LABID</t>
   </si>
@@ -2414,7 +2426,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3256,11 +3268,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H787"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A559" workbookViewId="0">
-      <selection activeCell="A576" sqref="A576"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3811,7 +3823,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -3837,7 +3849,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>498</v>
       </c>
@@ -3863,7 +3875,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -3889,7 +3901,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -3915,7 +3927,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -3941,7 +3953,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>509</v>
       </c>
@@ -3967,7 +3979,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -3993,7 +4005,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -4019,7 +4031,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -4045,7 +4057,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -4228,28 +4240,28 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+      <c r="A38" t="s">
         <v>199</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="2">
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38">
         <v>1</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="2">
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38">
         <v>186</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38">
         <v>283</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4461,29 +4473,29 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>605</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="1">
+      <c r="B47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="2">
         <v>1</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G47" s="1">
+      <c r="D47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" s="2">
         <v>322</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H47" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5060,54 +5072,54 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
+      <c r="A70" t="s">
         <v>39</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C70" s="2">
+      <c r="B70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70">
         <v>2</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" s="2">
+      <c r="D70" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70">
         <v>127</v>
       </c>
-      <c r="G70" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H70" s="2">
+      <c r="G70" t="s">
+        <v>9</v>
+      </c>
+      <c r="H70">
         <v>319</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
+      <c r="A71" t="s">
         <v>148</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C71" s="2">
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71">
         <v>1</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F71" s="2">
+      <c r="D71" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71">
         <v>233</v>
       </c>
-      <c r="G71" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H71" s="2">
+      <c r="G71" t="s">
+        <v>9</v>
+      </c>
+      <c r="H71">
         <v>332</v>
       </c>
     </row>
@@ -23736,11 +23748,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23888,31 +23900,31 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>518</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6">
         <v>321</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="2" t="s">
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
         <v>795</v>
       </c>
     </row>
@@ -24235,114 +24247,111 @@
         <v>795</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>559</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18">
         <v>10</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="2">
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18">
         <v>308</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="2" t="s">
+      <c r="H18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="1">
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2">
         <v>1</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="1">
+      <c r="D19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="2">
         <v>328</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I19" s="1" t="s">
+      <c r="G19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>795</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="1">
-        <v>319</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>795</v>
+      <c r="A20" t="s">
+        <v>561</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>310</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>562</v>
+        <v>263</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="1">
-        <v>309</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="1">
-        <v>327</v>
+      <c r="E21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="1">
+        <v>319</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>9</v>
@@ -24352,55 +24361,55 @@
       </c>
     </row>
     <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2">
+        <v>4</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2">
+        <v>309</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="2">
+        <v>327</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="1">
+      <c r="B23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="1">
         <v>4</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="1">
+      <c r="D23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="1">
         <v>294</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="1">
-        <v>29</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="1">
-        <v>320</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>9</v>
@@ -24409,15 +24418,15 @@
         <v>795</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>584</v>
+        <v>571</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="1">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>9</v>
@@ -24429,7 +24438,7 @@
         <v>9</v>
       </c>
       <c r="G24" s="1">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>9</v>
@@ -24438,15 +24447,15 @@
         <v>795</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>603</v>
+        <v>584</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>9</v>
@@ -24458,7 +24467,7 @@
         <v>9</v>
       </c>
       <c r="G25" s="1">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>9</v>
@@ -24467,15 +24476,15 @@
         <v>795</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>9</v>
@@ -24487,7 +24496,7 @@
         <v>9</v>
       </c>
       <c r="G26" s="1">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>9</v>
@@ -24497,153 +24506,150 @@
       </c>
     </row>
     <row r="27" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="2">
+        <v>322</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>606</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>272</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="1">
+      <c r="B29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="1">
         <v>1</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="1">
+      <c r="D29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="1">
         <v>326</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I27" s="1" t="s">
+      <c r="G29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>264</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="2">
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30">
         <v>47</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="2">
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30">
         <v>319</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I28" s="2" t="s">
+      <c r="G30" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>624</v>
       </c>
-      <c r="B29" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29">
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31">
         <v>291</v>
       </c>
-      <c r="D29" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H29" t="s">
-        <v>9</v>
-      </c>
-      <c r="I29" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="1">
-        <v>307</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="1">
-        <v>325</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I31" s="1" t="s">
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" t="s">
         <v>795</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>310</v>
+        <v>243</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>9</v>
@@ -24658,7 +24664,7 @@
         <v>9</v>
       </c>
       <c r="F32" s="1">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>9</v>
@@ -24672,13 +24678,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="1">
-        <v>1</v>
+      <c r="C33" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>9</v>
@@ -24687,7 +24693,7 @@
         <v>9</v>
       </c>
       <c r="F33" s="1">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>9</v>
@@ -24701,13 +24707,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>652</v>
+        <v>310</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>9</v>
@@ -24715,11 +24721,11 @@
       <c r="E34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G34" s="1">
-        <v>314</v>
+      <c r="F34" s="1">
+        <v>325</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>9</v>
@@ -24730,13 +24736,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>662</v>
+        <v>326</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C35" s="1">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>9</v>
@@ -24744,11 +24750,11 @@
       <c r="E35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" s="1">
-        <v>288</v>
+      <c r="F35" s="1">
+        <v>326</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>9</v>
@@ -24759,13 +24765,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>328</v>
+        <v>652</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C36" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>9</v>
@@ -24773,11 +24779,11 @@
       <c r="E36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="1">
-        <v>326</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>9</v>
+      <c r="F36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="1">
+        <v>314</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>9</v>
@@ -24788,13 +24794,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>380</v>
+        <v>662</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>9</v>
@@ -24802,11 +24808,11 @@
       <c r="E37" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="1">
-        <v>331</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>9</v>
+      <c r="F37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="1">
+        <v>288</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>9</v>
@@ -24816,130 +24822,130 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="1">
+        <v>326</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="1">
+        <v>45</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="1">
+        <v>331</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>314</v>
       </c>
-      <c r="B38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38">
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40">
         <v>250</v>
       </c>
-      <c r="D38" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38">
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40">
         <v>325</v>
       </c>
-      <c r="G38" t="s">
-        <v>9</v>
-      </c>
-      <c r="H38" t="s">
-        <v>9</v>
-      </c>
-      <c r="I38" t="s">
+      <c r="G40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>305</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="2">
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41">
         <v>41</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="2">
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41">
         <v>324</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="1">
-        <v>7</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="1">
-        <v>299</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>717</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="1">
-        <v>19</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="1">
-        <v>283</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I41" s="1" t="s">
+      <c r="G41" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" t="s">
         <v>795</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>367</v>
+        <v>230</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>9</v>
@@ -24948,7 +24954,7 @@
         <v>9</v>
       </c>
       <c r="F42" s="1">
-        <v>329</v>
+        <v>299</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>9</v>
@@ -24962,13 +24968,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>278</v>
+        <v>717</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>9</v>
+      <c r="C43" s="1">
+        <v>19</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>9</v>
@@ -24976,11 +24982,11 @@
       <c r="E43" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="1">
-        <v>321</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>9</v>
+      <c r="F43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" s="1">
+        <v>283</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>9</v>
@@ -24989,9 +24995,67 @@
         <v>795</v>
       </c>
     </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="1">
+        <v>329</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="1">
+        <v>321</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>795</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I42">
-    <sortCondition ref="I2:I42"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I44">
+    <sortCondition ref="I2:I44"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>